<commit_message>
Update Template Excel files to not contain extra line breaks
</commit_message>
<xml_diff>
--- a/lib/Template.xlsx
+++ b/lib/Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\luke\SwimifyHandler\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846FE66F-12E2-4341-9C4B-277FAA508751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927DC08F-2207-4259-9402-5EC1DDE60E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15345" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Empty" sheetId="4" r:id="rId1"/>
@@ -52,15 +52,6 @@
     <t>Tävlingsschema</t>
   </si>
   <si>
-    <t>SK Poseidon</t>
-  </si>
-  <si>
-    <t>Poseidon Team Cup</t>
-  </si>
-  <si>
-    <t>30 Augusti - 1 September (2024)</t>
-  </si>
-  <si>
     <t>$event$</t>
   </si>
   <si>
@@ -191,6 +182,15 @@
   </si>
   <si>
     <t>30. 50m</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>Swedish Swim Games 2024 - GP</t>
+  </si>
+  <si>
+    <t>20 September - 22 September (2024)</t>
   </si>
 </sst>
 </file>
@@ -1026,26 +1026,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{957E72E0-1634-4119-98B9-1FB2CF4FDFCD}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9" style="28"/>
+    <col min="1" max="8" width="9.625" style="28" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="9.9499999999999993" customHeight="1">
       <c r="A1" s="29" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
       <c r="D1" s="29" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="F1" s="29"/>
       <c r="G1" s="29"/>
@@ -1068,10 +1069,10 @@
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
       <c r="D3" s="29" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
@@ -1103,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB965E0-7BEE-4501-B7F4-BE32C71BF8BA}">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1120,34 +1121,34 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -1160,19 +1161,19 @@
     <row r="4" spans="1:8" ht="36" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="F4" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>0</v>
@@ -1181,7 +1182,7 @@
     </row>
     <row r="5" spans="1:8" ht="36" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="14"/>
@@ -1222,18 +1223,6 @@
       <c r="G9" s="9"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" ht="36" customHeight="1"/>
-    <row r="11" spans="1:8" ht="36" customHeight="1"/>
-    <row r="12" spans="1:8" ht="36" customHeight="1"/>
-    <row r="13" spans="1:8" ht="36" customHeight="1"/>
-    <row r="14" spans="1:8" ht="36" customHeight="1"/>
-    <row r="15" spans="1:8" ht="36" customHeight="1"/>
-    <row r="16" spans="1:8" ht="36" customHeight="1"/>
-    <row r="17" ht="36" customHeight="1"/>
-    <row r="18" ht="36" customHeight="1"/>
-    <row r="19" ht="36" customHeight="1"/>
-    <row r="20" ht="36" customHeight="1"/>
-    <row r="21" ht="36" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1242,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0908E2-138E-4E2B-903F-6A8AC635D76F}">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A10" sqref="A10:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1259,34 +1248,34 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -1299,19 +1288,19 @@
     <row r="4" spans="1:8" ht="36" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="F4" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>0</v>
@@ -1361,18 +1350,6 @@
       <c r="G9" s="9"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" ht="36" customHeight="1"/>
-    <row r="11" spans="1:8" ht="36" customHeight="1"/>
-    <row r="12" spans="1:8" ht="36" customHeight="1"/>
-    <row r="13" spans="1:8" ht="36" customHeight="1"/>
-    <row r="14" spans="1:8" ht="36" customHeight="1"/>
-    <row r="15" spans="1:8" ht="36" customHeight="1"/>
-    <row r="16" spans="1:8" ht="36" customHeight="1"/>
-    <row r="17" ht="36" customHeight="1"/>
-    <row r="18" ht="36" customHeight="1"/>
-    <row r="19" ht="36" customHeight="1"/>
-    <row r="20" ht="36" customHeight="1"/>
-    <row r="21" ht="36" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1381,10 +1358,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1A2F7B-8CAA-422F-9A29-95EA4DAD8CCD}">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1398,34 +1375,34 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -1438,19 +1415,19 @@
     <row r="4" spans="1:8" ht="36" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="F4" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>0</v>
@@ -1459,7 +1436,7 @@
     </row>
     <row r="5" spans="1:8" ht="36" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="13"/>
@@ -1512,18 +1489,6 @@
       <c r="G10" s="9"/>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8" ht="36" customHeight="1"/>
-    <row r="12" spans="1:8" ht="36" customHeight="1"/>
-    <row r="13" spans="1:8" ht="36" customHeight="1"/>
-    <row r="14" spans="1:8" ht="36" customHeight="1"/>
-    <row r="15" spans="1:8" ht="36" customHeight="1"/>
-    <row r="16" spans="1:8" ht="36" customHeight="1"/>
-    <row r="17" ht="36" customHeight="1"/>
-    <row r="18" ht="36" customHeight="1"/>
-    <row r="19" ht="36" customHeight="1"/>
-    <row r="20" ht="36" customHeight="1"/>
-    <row r="21" ht="36" customHeight="1"/>
-    <row r="22" ht="36" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1531,10 +1496,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394A3B2C-3024-44D3-BF6A-3F4279E7F853}">
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1548,34 +1513,34 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -1588,19 +1553,19 @@
     <row r="4" spans="1:8" ht="36" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="F4" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>0</v>
@@ -1686,18 +1651,6 @@
       <c r="G12" s="9"/>
       <c r="H12" s="10"/>
     </row>
-    <row r="13" spans="1:8" ht="36" customHeight="1"/>
-    <row r="14" spans="1:8" ht="36" customHeight="1"/>
-    <row r="15" spans="1:8" ht="36" customHeight="1"/>
-    <row r="16" spans="1:8" ht="36" customHeight="1"/>
-    <row r="17" ht="36" customHeight="1"/>
-    <row r="18" ht="36" customHeight="1"/>
-    <row r="19" ht="36" customHeight="1"/>
-    <row r="20" ht="36" customHeight="1"/>
-    <row r="21" ht="36" customHeight="1"/>
-    <row r="22" ht="36" customHeight="1"/>
-    <row r="23" ht="36" customHeight="1"/>
-    <row r="24" ht="36" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1705,10 +1658,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B71A937-E5C0-4E0D-A132-3B229F2F7A7B}">
-  <dimension ref="A1:W28"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1722,34 +1675,34 @@
   <sheetData>
     <row r="1" spans="1:23" ht="18" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="18" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -1762,19 +1715,19 @@
     <row r="4" spans="1:23" ht="36" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="F4" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>0</v>
@@ -1843,7 +1796,7 @@
     </row>
     <row r="9" spans="1:23" customFormat="1" ht="36" customHeight="1">
       <c r="A9" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="13"/>
@@ -1861,7 +1814,7 @@
     </row>
     <row r="10" spans="1:23" customFormat="1" ht="36" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="13"/>
@@ -1879,7 +1832,7 @@
     </row>
     <row r="11" spans="1:23" customFormat="1" ht="36" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="13"/>
@@ -1897,7 +1850,7 @@
     </row>
     <row r="12" spans="1:23" customFormat="1" ht="36" customHeight="1">
       <c r="A12" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="14"/>
@@ -1977,214 +1930,6 @@
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="1:23" customFormat="1" ht="36" customHeight="1">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="2"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
-    </row>
-    <row r="18" spans="1:23" customFormat="1" ht="36" customHeight="1">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="2"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-    </row>
-    <row r="19" spans="1:23" customFormat="1" ht="36" customHeight="1">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="2"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-    </row>
-    <row r="20" spans="1:23" customFormat="1" ht="36" customHeight="1">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="2"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-    </row>
-    <row r="21" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H21" s="2"/>
-      <c r="I21"/>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21"/>
-      <c r="O21"/>
-      <c r="P21"/>
-      <c r="Q21"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-    </row>
-    <row r="22" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H22" s="2"/>
-      <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22"/>
-      <c r="L22"/>
-      <c r="M22"/>
-      <c r="N22"/>
-      <c r="O22"/>
-      <c r="P22"/>
-      <c r="Q22"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-    </row>
-    <row r="23" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H23" s="2"/>
-      <c r="I23"/>
-      <c r="J23"/>
-      <c r="K23"/>
-      <c r="L23"/>
-      <c r="M23"/>
-      <c r="N23"/>
-      <c r="O23"/>
-      <c r="P23"/>
-      <c r="Q23"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-    </row>
-    <row r="24" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H24" s="2"/>
-      <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-      <c r="M24"/>
-      <c r="N24"/>
-      <c r="O24"/>
-      <c r="P24"/>
-      <c r="Q24"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-    </row>
-    <row r="25" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H25" s="2"/>
-      <c r="I25"/>
-      <c r="J25"/>
-      <c r="K25"/>
-      <c r="L25"/>
-      <c r="M25"/>
-      <c r="N25"/>
-      <c r="O25"/>
-      <c r="P25"/>
-      <c r="Q25"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-    </row>
-    <row r="26" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H26" s="2"/>
-      <c r="I26"/>
-      <c r="J26"/>
-      <c r="K26"/>
-      <c r="L26"/>
-      <c r="M26"/>
-      <c r="N26"/>
-      <c r="O26"/>
-      <c r="P26"/>
-      <c r="Q26"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-    </row>
-    <row r="27" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H27" s="2"/>
-      <c r="I27"/>
-      <c r="J27"/>
-      <c r="K27"/>
-      <c r="L27"/>
-      <c r="M27"/>
-      <c r="N27"/>
-      <c r="O27"/>
-      <c r="P27"/>
-      <c r="Q27"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-    </row>
-    <row r="28" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H28" s="2"/>
-      <c r="I28"/>
-      <c r="J28"/>
-      <c r="K28"/>
-      <c r="L28"/>
-      <c r="M28"/>
-      <c r="N28"/>
-      <c r="O28"/>
-      <c r="P28"/>
-      <c r="Q28"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2192,10 +1937,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A43102-E64B-4A1B-B802-53C904565E43}">
-  <dimension ref="A1:W36"/>
+  <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2209,34 +1954,34 @@
   <sheetData>
     <row r="1" spans="1:23" ht="18" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="18" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -2249,19 +1994,19 @@
     <row r="4" spans="1:23" ht="36" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="F4" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>0</v>
@@ -2318,7 +2063,7 @@
     </row>
     <row r="9" spans="1:23" ht="36" customHeight="1">
       <c r="A9" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="13"/>
@@ -2330,7 +2075,7 @@
     </row>
     <row r="10" spans="1:23" ht="36" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="13"/>
@@ -2342,7 +2087,7 @@
     </row>
     <row r="11" spans="1:23" ht="36" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="13"/>
@@ -2354,7 +2099,7 @@
     </row>
     <row r="12" spans="1:23" ht="36" customHeight="1">
       <c r="A12" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="13"/>
@@ -2366,7 +2111,7 @@
     </row>
     <row r="13" spans="1:23" ht="36" customHeight="1">
       <c r="A13" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="13"/>
@@ -2378,7 +2123,7 @@
     </row>
     <row r="14" spans="1:23" ht="36" customHeight="1">
       <c r="A14" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="13"/>
@@ -2390,7 +2135,7 @@
     </row>
     <row r="15" spans="1:23" customFormat="1" ht="36" customHeight="1">
       <c r="A15" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="13"/>
@@ -2408,7 +2153,7 @@
     </row>
     <row r="16" spans="1:23" customFormat="1" ht="36" customHeight="1">
       <c r="A16" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="13"/>
@@ -2426,7 +2171,7 @@
     </row>
     <row r="17" spans="1:23" customFormat="1" ht="36" customHeight="1">
       <c r="A17" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="13"/>
@@ -2444,7 +2189,7 @@
     </row>
     <row r="18" spans="1:23" customFormat="1" ht="36" customHeight="1">
       <c r="A18" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="13"/>
@@ -2462,7 +2207,7 @@
     </row>
     <row r="19" spans="1:23" customFormat="1" ht="36" customHeight="1">
       <c r="A19" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="13"/>
@@ -2480,7 +2225,7 @@
     </row>
     <row r="20" spans="1:23" customFormat="1" ht="36" customHeight="1">
       <c r="A20" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B20" s="16"/>
       <c r="C20" s="14"/>
@@ -2560,214 +2305,6 @@
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
     </row>
-    <row r="25" spans="1:23" customFormat="1" ht="36" customHeight="1">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="2"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-    </row>
-    <row r="26" spans="1:23" customFormat="1" ht="36" customHeight="1">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="2"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-    </row>
-    <row r="27" spans="1:23" customFormat="1" ht="36" customHeight="1">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="2"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-    </row>
-    <row r="28" spans="1:23" customFormat="1" ht="36" customHeight="1">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="2"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-    </row>
-    <row r="29" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H29" s="2"/>
-      <c r="I29"/>
-      <c r="J29"/>
-      <c r="K29"/>
-      <c r="L29"/>
-      <c r="M29"/>
-      <c r="N29"/>
-      <c r="O29"/>
-      <c r="P29"/>
-      <c r="Q29"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-    </row>
-    <row r="30" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H30" s="2"/>
-      <c r="I30"/>
-      <c r="J30"/>
-      <c r="K30"/>
-      <c r="L30"/>
-      <c r="M30"/>
-      <c r="N30"/>
-      <c r="O30"/>
-      <c r="P30"/>
-      <c r="Q30"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
-    </row>
-    <row r="31" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H31" s="2"/>
-      <c r="I31"/>
-      <c r="J31"/>
-      <c r="K31"/>
-      <c r="L31"/>
-      <c r="M31"/>
-      <c r="N31"/>
-      <c r="O31"/>
-      <c r="P31"/>
-      <c r="Q31"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-      <c r="T31" s="1"/>
-      <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
-      <c r="W31" s="1"/>
-    </row>
-    <row r="32" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H32" s="2"/>
-      <c r="I32"/>
-      <c r="J32"/>
-      <c r="K32"/>
-      <c r="L32"/>
-      <c r="M32"/>
-      <c r="N32"/>
-      <c r="O32"/>
-      <c r="P32"/>
-      <c r="Q32"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
-      <c r="T32" s="1"/>
-      <c r="U32" s="1"/>
-      <c r="V32" s="1"/>
-      <c r="W32" s="1"/>
-    </row>
-    <row r="33" spans="8:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H33" s="2"/>
-      <c r="I33"/>
-      <c r="J33"/>
-      <c r="K33"/>
-      <c r="L33"/>
-      <c r="M33"/>
-      <c r="N33"/>
-      <c r="O33"/>
-      <c r="P33"/>
-      <c r="Q33"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
-      <c r="U33" s="1"/>
-      <c r="V33" s="1"/>
-      <c r="W33" s="1"/>
-    </row>
-    <row r="34" spans="8:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H34" s="2"/>
-      <c r="I34"/>
-      <c r="J34"/>
-      <c r="K34"/>
-      <c r="L34"/>
-      <c r="M34"/>
-      <c r="N34"/>
-      <c r="O34"/>
-      <c r="P34"/>
-      <c r="Q34"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-      <c r="T34" s="1"/>
-      <c r="U34" s="1"/>
-      <c r="V34" s="1"/>
-      <c r="W34" s="1"/>
-    </row>
-    <row r="35" spans="8:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H35" s="2"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35"/>
-      <c r="M35"/>
-      <c r="N35"/>
-      <c r="O35"/>
-      <c r="P35"/>
-      <c r="Q35"/>
-      <c r="R35" s="1"/>
-      <c r="S35" s="1"/>
-      <c r="T35" s="1"/>
-      <c r="U35" s="1"/>
-      <c r="V35" s="1"/>
-      <c r="W35" s="1"/>
-    </row>
-    <row r="36" spans="8:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H36" s="2"/>
-      <c r="I36"/>
-      <c r="J36"/>
-      <c r="K36"/>
-      <c r="L36"/>
-      <c r="M36"/>
-      <c r="N36"/>
-      <c r="O36"/>
-      <c r="P36"/>
-      <c r="Q36"/>
-      <c r="R36" s="1"/>
-      <c r="S36" s="1"/>
-      <c r="T36" s="1"/>
-      <c r="U36" s="1"/>
-      <c r="V36" s="1"/>
-      <c r="W36" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2775,10 +2312,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C0F73C-1FF2-41CB-91C1-CBBCDB3326E9}">
-  <dimension ref="A1:W50"/>
+  <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2792,34 +2329,34 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -2832,19 +2369,19 @@
     <row r="4" spans="1:8" ht="36" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="F4" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>0</v>
@@ -2901,7 +2438,7 @@
     </row>
     <row r="9" spans="1:8" ht="36" customHeight="1">
       <c r="A9" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="13"/>
@@ -2913,7 +2450,7 @@
     </row>
     <row r="10" spans="1:8" ht="36" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="13"/>
@@ -2925,7 +2462,7 @@
     </row>
     <row r="11" spans="1:8" ht="36" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="13"/>
@@ -2937,7 +2474,7 @@
     </row>
     <row r="12" spans="1:8" ht="36" customHeight="1">
       <c r="A12" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="13"/>
@@ -2949,7 +2486,7 @@
     </row>
     <row r="13" spans="1:8" ht="36" customHeight="1">
       <c r="A13" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="13"/>
@@ -2961,7 +2498,7 @@
     </row>
     <row r="14" spans="1:8" ht="36" customHeight="1">
       <c r="A14" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="13"/>
@@ -2973,7 +2510,7 @@
     </row>
     <row r="15" spans="1:8" ht="36" customHeight="1">
       <c r="A15" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="13"/>
@@ -2985,7 +2522,7 @@
     </row>
     <row r="16" spans="1:8" ht="36" customHeight="1">
       <c r="A16" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="13"/>
@@ -2997,7 +2534,7 @@
     </row>
     <row r="17" spans="1:23" ht="36" customHeight="1">
       <c r="A17" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="13"/>
@@ -3009,7 +2546,7 @@
     </row>
     <row r="18" spans="1:23" ht="36" customHeight="1">
       <c r="A18" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="13"/>
@@ -3021,7 +2558,7 @@
     </row>
     <row r="19" spans="1:23" ht="36" customHeight="1">
       <c r="A19" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="13"/>
@@ -3033,7 +2570,7 @@
     </row>
     <row r="20" spans="1:23" ht="36" customHeight="1">
       <c r="A20" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="13"/>
@@ -3045,7 +2582,7 @@
     </row>
     <row r="21" spans="1:23" ht="36" customHeight="1">
       <c r="A21" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="13"/>
@@ -3057,7 +2594,7 @@
     </row>
     <row r="22" spans="1:23" ht="36" customHeight="1">
       <c r="A22" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="13"/>
@@ -3069,7 +2606,7 @@
     </row>
     <row r="23" spans="1:23" ht="36" customHeight="1">
       <c r="A23" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="13"/>
@@ -3081,7 +2618,7 @@
     </row>
     <row r="24" spans="1:23" ht="36" customHeight="1">
       <c r="A24" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="13"/>
@@ -3093,7 +2630,7 @@
     </row>
     <row r="25" spans="1:23" ht="36" customHeight="1">
       <c r="A25" s="11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="13"/>
@@ -3105,7 +2642,7 @@
     </row>
     <row r="26" spans="1:23" ht="36" customHeight="1">
       <c r="A26" s="11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="13"/>
@@ -3117,7 +2654,7 @@
     </row>
     <row r="27" spans="1:23" ht="36" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="13"/>
@@ -3129,7 +2666,7 @@
     </row>
     <row r="28" spans="1:23" ht="36" customHeight="1">
       <c r="A28" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="13"/>
@@ -3141,7 +2678,7 @@
     </row>
     <row r="29" spans="1:23" customFormat="1" ht="36" customHeight="1">
       <c r="A29" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="13"/>
@@ -3159,7 +2696,7 @@
     </row>
     <row r="30" spans="1:23" customFormat="1" ht="36" customHeight="1">
       <c r="A30" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="13"/>
@@ -3177,7 +2714,7 @@
     </row>
     <row r="31" spans="1:23" customFormat="1" ht="36" customHeight="1">
       <c r="A31" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="13"/>
@@ -3195,7 +2732,7 @@
     </row>
     <row r="32" spans="1:23" customFormat="1" ht="36" customHeight="1">
       <c r="A32" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="13"/>
@@ -3213,7 +2750,7 @@
     </row>
     <row r="33" spans="1:23" customFormat="1" ht="36" customHeight="1">
       <c r="A33" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="13"/>
@@ -3231,7 +2768,7 @@
     </row>
     <row r="34" spans="1:23" customFormat="1" ht="36" customHeight="1">
       <c r="A34" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B34" s="16"/>
       <c r="C34" s="14"/>
@@ -3311,214 +2848,6 @@
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
     </row>
-    <row r="39" spans="1:23" customFormat="1" ht="36" customHeight="1">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="2"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="1"/>
-      <c r="T39" s="1"/>
-      <c r="U39" s="1"/>
-      <c r="V39" s="1"/>
-      <c r="W39" s="1"/>
-    </row>
-    <row r="40" spans="1:23" customFormat="1" ht="36" customHeight="1">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="2"/>
-      <c r="R40" s="1"/>
-      <c r="S40" s="1"/>
-      <c r="T40" s="1"/>
-      <c r="U40" s="1"/>
-      <c r="V40" s="1"/>
-      <c r="W40" s="1"/>
-    </row>
-    <row r="41" spans="1:23" customFormat="1" ht="36" customHeight="1">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="2"/>
-      <c r="R41" s="1"/>
-      <c r="S41" s="1"/>
-      <c r="T41" s="1"/>
-      <c r="U41" s="1"/>
-      <c r="V41" s="1"/>
-      <c r="W41" s="1"/>
-    </row>
-    <row r="42" spans="1:23" customFormat="1" ht="36" customHeight="1">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="2"/>
-      <c r="R42" s="1"/>
-      <c r="S42" s="1"/>
-      <c r="T42" s="1"/>
-      <c r="U42" s="1"/>
-      <c r="V42" s="1"/>
-      <c r="W42" s="1"/>
-    </row>
-    <row r="43" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H43" s="2"/>
-      <c r="I43"/>
-      <c r="J43"/>
-      <c r="K43"/>
-      <c r="L43"/>
-      <c r="M43"/>
-      <c r="N43"/>
-      <c r="O43"/>
-      <c r="P43"/>
-      <c r="Q43"/>
-      <c r="R43" s="1"/>
-      <c r="S43" s="1"/>
-      <c r="T43" s="1"/>
-      <c r="U43" s="1"/>
-      <c r="V43" s="1"/>
-      <c r="W43" s="1"/>
-    </row>
-    <row r="44" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H44" s="2"/>
-      <c r="I44"/>
-      <c r="J44"/>
-      <c r="K44"/>
-      <c r="L44"/>
-      <c r="M44"/>
-      <c r="N44"/>
-      <c r="O44"/>
-      <c r="P44"/>
-      <c r="Q44"/>
-      <c r="R44" s="1"/>
-      <c r="S44" s="1"/>
-      <c r="T44" s="1"/>
-      <c r="U44" s="1"/>
-      <c r="V44" s="1"/>
-      <c r="W44" s="1"/>
-    </row>
-    <row r="45" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H45" s="2"/>
-      <c r="I45"/>
-      <c r="J45"/>
-      <c r="K45"/>
-      <c r="L45"/>
-      <c r="M45"/>
-      <c r="N45"/>
-      <c r="O45"/>
-      <c r="P45"/>
-      <c r="Q45"/>
-      <c r="R45" s="1"/>
-      <c r="S45" s="1"/>
-      <c r="T45" s="1"/>
-      <c r="U45" s="1"/>
-      <c r="V45" s="1"/>
-      <c r="W45" s="1"/>
-    </row>
-    <row r="46" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H46" s="2"/>
-      <c r="I46"/>
-      <c r="J46"/>
-      <c r="K46"/>
-      <c r="L46"/>
-      <c r="M46"/>
-      <c r="N46"/>
-      <c r="O46"/>
-      <c r="P46"/>
-      <c r="Q46"/>
-      <c r="R46" s="1"/>
-      <c r="S46" s="1"/>
-      <c r="T46" s="1"/>
-      <c r="U46" s="1"/>
-      <c r="V46" s="1"/>
-      <c r="W46" s="1"/>
-    </row>
-    <row r="47" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H47" s="2"/>
-      <c r="I47"/>
-      <c r="J47"/>
-      <c r="K47"/>
-      <c r="L47"/>
-      <c r="M47"/>
-      <c r="N47"/>
-      <c r="O47"/>
-      <c r="P47"/>
-      <c r="Q47"/>
-      <c r="R47" s="1"/>
-      <c r="S47" s="1"/>
-      <c r="T47" s="1"/>
-      <c r="U47" s="1"/>
-      <c r="V47" s="1"/>
-      <c r="W47" s="1"/>
-    </row>
-    <row r="48" spans="1:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H48" s="2"/>
-      <c r="I48"/>
-      <c r="J48"/>
-      <c r="K48"/>
-      <c r="L48"/>
-      <c r="M48"/>
-      <c r="N48"/>
-      <c r="O48"/>
-      <c r="P48"/>
-      <c r="Q48"/>
-      <c r="R48" s="1"/>
-      <c r="S48" s="1"/>
-      <c r="T48" s="1"/>
-      <c r="U48" s="1"/>
-      <c r="V48" s="1"/>
-      <c r="W48" s="1"/>
-    </row>
-    <row r="49" spans="8:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H49" s="2"/>
-      <c r="I49"/>
-      <c r="J49"/>
-      <c r="K49"/>
-      <c r="L49"/>
-      <c r="M49"/>
-      <c r="N49"/>
-      <c r="O49"/>
-      <c r="P49"/>
-      <c r="Q49"/>
-      <c r="R49" s="1"/>
-      <c r="S49" s="1"/>
-      <c r="T49" s="1"/>
-      <c r="U49" s="1"/>
-      <c r="V49" s="1"/>
-      <c r="W49" s="1"/>
-    </row>
-    <row r="50" spans="8:23" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="H50" s="2"/>
-      <c r="I50"/>
-      <c r="J50"/>
-      <c r="K50"/>
-      <c r="L50"/>
-      <c r="M50"/>
-      <c r="N50"/>
-      <c r="O50"/>
-      <c r="P50"/>
-      <c r="Q50"/>
-      <c r="R50" s="1"/>
-      <c r="S50" s="1"/>
-      <c r="T50" s="1"/>
-      <c r="U50" s="1"/>
-      <c r="V50" s="1"/>
-      <c r="W50" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>